<commit_message>
Worked on the master micro controller
</commit_message>
<xml_diff>
--- a/Projektbericht.xlsx
+++ b/Projektbericht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffaiku/opt/FH/Embeded Systems/Projekt/smart_traffic_light/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C05BCB-ED13-4B46-ADE0-50EF3B75BF80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE42BA6A-4F79-144D-A11C-D0879117A26E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="1500" windowWidth="28240" windowHeight="17560" xr2:uid="{93A82D61-4F1F-7040-9F2C-9B98C5ACB1F6}"/>
   </bookViews>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FDA282-4BD6-4647-9C33-15F51F20F28F}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,19 +554,24 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1">
-        <f>SUM(B2:B10)</f>
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <f>SUM(D2:D10)</f>
-        <v>2</v>
-      </c>
-      <c r="F13" s="1">
-        <f>SUM(F2:F10)</f>
+      <c r="B36">
+        <f>SUM(B2:B35)</f>
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <f>SUM(D2:D35)</f>
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <f>SUM(F2:F35)</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>